<commit_message>
Update SECURDE MP - Access Matrix v3.0.xlsx
</commit_message>
<xml_diff>
--- a/SECURDE MP - Access Matrix v3.0.xlsx
+++ b/SECURDE MP - Access Matrix v3.0.xlsx
@@ -1,62 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="22202"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Norielle\Desktop\School\DLSU\securde-mco2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F49C1FB-59DF-43A1-A51B-8C6AD8BA4AE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14880" tabRatio="717" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Student G301</author>
-  </authors>
-  <commentList>
-    <comment ref="D2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Sir Fritz</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-SAMPLE ONLY :)</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="133">
   <si>
     <t>ACCESS MATRIX</t>
   </si>
@@ -68,33 +40,6 @@
   </si>
   <si>
     <t>Login</t>
-  </si>
-  <si>
-    <t>FUNC2</t>
-  </si>
-  <si>
-    <t>FUNC3</t>
-  </si>
-  <si>
-    <t>FUNC4</t>
-  </si>
-  <si>
-    <t>FUNC5</t>
-  </si>
-  <si>
-    <t>FUNC6</t>
-  </si>
-  <si>
-    <t>FUNC7</t>
-  </si>
-  <si>
-    <t>FUNC8</t>
-  </si>
-  <si>
-    <t>FUNC9</t>
-  </si>
-  <si>
-    <t>FUNC10</t>
   </si>
   <si>
     <t>Unregistered</t>
@@ -121,43 +66,10 @@
     <t>Disabled</t>
   </si>
   <si>
-    <t>User - Search</t>
-  </si>
-  <si>
-    <t>Only able to search Client users</t>
-  </si>
-  <si>
-    <t>Only able to search Client and Staff Users</t>
-  </si>
-  <si>
     <t>FULL Function</t>
   </si>
   <si>
     <t>Partial Function</t>
-  </si>
-  <si>
-    <t>FUNC11</t>
-  </si>
-  <si>
-    <t>FUNC12</t>
-  </si>
-  <si>
-    <t>FUNC13</t>
-  </si>
-  <si>
-    <t>FUNC14</t>
-  </si>
-  <si>
-    <t>FUNC15</t>
-  </si>
-  <si>
-    <t>FUNC16</t>
-  </si>
-  <si>
-    <t>FUNC17</t>
-  </si>
-  <si>
-    <t>FUNC18</t>
   </si>
   <si>
     <t>FUNC19</t>
@@ -457,12 +369,82 @@
   <si>
     <t>n/a</t>
   </si>
+  <si>
+    <t>User Tab</t>
+  </si>
+  <si>
+    <t>Products - Add</t>
+  </si>
+  <si>
+    <t>add same products</t>
+  </si>
+  <si>
+    <t>Products - Purchase stock</t>
+  </si>
+  <si>
+    <t>Only able to search products bought by the user</t>
+  </si>
+  <si>
+    <t>History - Search</t>
+  </si>
+  <si>
+    <t>History - Reload</t>
+  </si>
+  <si>
+    <t>History Tab</t>
+  </si>
+  <si>
+    <t>Products Tab</t>
+  </si>
+  <si>
+    <t>Products - Edit</t>
+  </si>
+  <si>
+    <t>Products - Delete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only able to see transactions of clients </t>
+  </si>
+  <si>
+    <t>Logs Tab</t>
+  </si>
+  <si>
+    <t>denial of service</t>
+  </si>
+  <si>
+    <t>reload must be disabled for 5s after clicking
+lockout system?</t>
+  </si>
+  <si>
+    <t>Cannot edit product names</t>
+  </si>
+  <si>
+    <t>Can only edit stock number (cannot input number less than current stocks)</t>
+  </si>
+  <si>
+    <t>Only able to see own transactions</t>
+  </si>
+  <si>
+    <t>Admin Home</t>
+  </si>
+  <si>
+    <t>Manager Home</t>
+  </si>
+  <si>
+    <t>Staff Home</t>
+  </si>
+  <si>
+    <t>Client Home</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -477,19 +459,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
@@ -519,6 +488,7 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -526,6 +496,7 @@
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -722,14 +693,14 @@
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -760,7 +731,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -802,33 +773,33 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1110,37 +1081,50 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:XFA19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="175" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="11" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" customWidth="1"/>
+    <col min="17" max="17" width="17" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" s="29" customFormat="1" ht="24" thickBot="1">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:16381" s="33" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16384" ht="15" thickBot="1">
+    <row r="2" spans="1:16381" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -1151,309 +1135,300 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
+      <c r="AA2" s="1" t="s">
+        <v>22</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
+      <c r="AB2" s="1" t="s">
+        <v>23</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>6</v>
+      <c r="AC2" s="1" t="s">
+        <v>24</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>7</v>
+      <c r="AD2" s="1" t="s">
+        <v>25</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="AK2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="AO2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="AP2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AQ2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AR2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AT2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AU2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AV2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AW2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AX2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AY2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AZ2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="BA2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="BB2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="BC2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="BD2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="BE2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AO2" s="1" t="s">
+      <c r="BF2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AP2" s="1" t="s">
+      <c r="BG2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AQ2" s="1" t="s">
+      <c r="BH2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AR2" s="1" t="s">
+      <c r="BI2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AS2" s="1" t="s">
+      <c r="BJ2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AT2" s="1" t="s">
+      <c r="BK2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="BL2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AV2" s="1" t="s">
+      <c r="BM2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="BN2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AX2" s="1" t="s">
+      <c r="BO2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AY2" s="1" t="s">
+      <c r="BP2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AZ2" s="1" t="s">
+      <c r="BQ2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BA2" s="1" t="s">
+      <c r="BR2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BB2" s="1" t="s">
+      <c r="BS2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BC2" s="1" t="s">
+      <c r="BT2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="BD2" s="1" t="s">
+      <c r="BU2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="BE2" s="1" t="s">
+      <c r="BV2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="BF2" s="1" t="s">
+      <c r="BW2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="BG2" s="1" t="s">
+      <c r="BX2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="BH2" s="1" t="s">
+      <c r="BY2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="BI2" s="1" t="s">
+      <c r="BZ2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="BJ2" s="1" t="s">
+      <c r="CA2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="BK2" s="1" t="s">
+      <c r="CB2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BL2" s="1" t="s">
+      <c r="CC2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="BM2" s="1" t="s">
+      <c r="CD2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="BN2" s="1" t="s">
+      <c r="CE2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="BO2" s="1" t="s">
+      <c r="CF2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="BP2" s="1" t="s">
+      <c r="CG2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="BQ2" s="1" t="s">
+      <c r="CH2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="BR2" s="1" t="s">
+      <c r="CI2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="BS2" s="1" t="s">
+      <c r="CJ2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="BT2" s="1" t="s">
+      <c r="CK2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="BU2" s="1" t="s">
+      <c r="CL2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="BV2" s="1" t="s">
+      <c r="CM2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="BW2" s="1" t="s">
+      <c r="CN2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="BX2" s="1" t="s">
+      <c r="CO2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="BY2" s="1" t="s">
+      <c r="CP2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="BZ2" s="1" t="s">
+      <c r="CQ2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="CA2" s="1" t="s">
+      <c r="CR2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="CB2" s="1" t="s">
+      <c r="CS2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="CC2" s="1" t="s">
+      <c r="CT2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="CD2" s="1" t="s">
+      <c r="CU2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="CE2" s="1" t="s">
+      <c r="CV2" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="CF2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="CG2" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="CH2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="CI2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="CJ2" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="CK2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="CL2" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="CM2" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="CN2" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="CO2" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="CP2" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="CQ2" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="CR2" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="CS2" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="CT2" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="CU2" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="CV2" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="CW2" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="CX2" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="CY2" s="2" t="s">
-        <v>115</v>
-      </c>
     </row>
-    <row r="3" spans="1:16384" ht="20" customHeight="1">
+    <row r="3" spans="1:16381" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="7"/>
@@ -1463,7 +1438,6 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
@@ -1553,14 +1527,11 @@
       <c r="CS3" s="7"/>
       <c r="CT3" s="7"/>
       <c r="CU3" s="7"/>
-      <c r="CV3" s="7"/>
-      <c r="CW3" s="7"/>
-      <c r="CX3" s="7"/>
-      <c r="CY3" s="9"/>
+      <c r="CV3" s="9"/>
     </row>
-    <row r="4" spans="1:16384" ht="20" customHeight="1">
+    <row r="4" spans="1:16381" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="7"/>
@@ -1570,7 +1541,6 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
@@ -1660,32 +1630,32 @@
       <c r="CS4" s="7"/>
       <c r="CT4" s="7"/>
       <c r="CU4" s="7"/>
-      <c r="CV4" s="7"/>
-      <c r="CW4" s="7"/>
-      <c r="CX4" s="7"/>
-      <c r="CY4" s="9"/>
+      <c r="CV4" s="9"/>
     </row>
-    <row r="5" spans="1:16384" ht="50" customHeight="1">
+    <row r="5" spans="1:16381" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="6"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
       <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
       <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
+      <c r="J5" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="L5" s="6"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
@@ -1767,34 +1737,30 @@
       <c r="CS5" s="7"/>
       <c r="CT5" s="7"/>
       <c r="CU5" s="7"/>
-      <c r="CV5" s="7"/>
-      <c r="CW5" s="7"/>
-      <c r="CX5" s="7"/>
-      <c r="CY5" s="9"/>
+      <c r="CV5" s="9"/>
     </row>
-    <row r="6" spans="1:16384" ht="50" customHeight="1">
+    <row r="6" spans="1:16381" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="7"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+      <c r="H6" s="10" t="s">
+        <v>126</v>
+      </c>
       <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
+      <c r="P6" s="6"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
+      <c r="R6" s="6"/>
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
       <c r="U6" s="7"/>
@@ -1876,34 +1842,33 @@
       <c r="CS6" s="7"/>
       <c r="CT6" s="7"/>
       <c r="CU6" s="7"/>
-      <c r="CV6" s="7"/>
-      <c r="CW6" s="7"/>
-      <c r="CX6" s="7"/>
-      <c r="CY6" s="9"/>
+      <c r="CV6" s="9"/>
     </row>
-    <row r="7" spans="1:16384" ht="50" customHeight="1">
+    <row r="7" spans="1:16381" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="6"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="H7" s="10" t="s">
+        <v>125</v>
+      </c>
       <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
+      <c r="J7" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
+      <c r="O7" s="6"/>
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
+      <c r="R7" s="6"/>
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
@@ -1985,32 +1950,28 @@
       <c r="CS7" s="7"/>
       <c r="CT7" s="7"/>
       <c r="CU7" s="7"/>
-      <c r="CV7" s="7"/>
-      <c r="CW7" s="7"/>
-      <c r="CX7" s="7"/>
-      <c r="CY7" s="9"/>
+      <c r="CV7" s="9"/>
     </row>
-    <row r="8" spans="1:16384" ht="50" customHeight="1" thickBot="1">
+    <row r="8" spans="1:16381" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
+      <c r="E8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
       <c r="O8" s="11"/>
       <c r="P8" s="11"/>
       <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
+      <c r="R8" s="6"/>
       <c r="S8" s="11"/>
       <c r="T8" s="11"/>
       <c r="U8" s="11"/>
@@ -2092,70 +2053,76 @@
       <c r="CS8" s="11"/>
       <c r="CT8" s="11"/>
       <c r="CU8" s="11"/>
-      <c r="CV8" s="11"/>
-      <c r="CW8" s="11"/>
-      <c r="CX8" s="11"/>
-      <c r="CY8" s="13"/>
+      <c r="CV8" s="13"/>
     </row>
-    <row r="9" spans="1:16384" s="25" customFormat="1" ht="15" thickBot="1"/>
-    <row r="10" spans="1:16384" s="32" customFormat="1" ht="45" customHeight="1" thickBot="1">
+    <row r="9" spans="1:16381" s="25" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:16381" s="31" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
-      <c r="B10" s="31" t="s">
-        <v>120</v>
+      <c r="B10" s="30" t="s">
+        <v>100</v>
       </c>
-      <c r="C10" s="31" t="s">
-        <v>122</v>
+      <c r="C10" s="30" t="s">
+        <v>102</v>
       </c>
-      <c r="D10" s="31" t="s">
-        <v>127</v>
+      <c r="D10" s="30" t="s">
+        <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:16384" s="27" customFormat="1" ht="45" customHeight="1" thickBot="1">
-      <c r="A11" s="33" t="s">
-        <v>117</v>
+    <row r="11" spans="1:16381" s="27" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="32" t="s">
+        <v>97</v>
       </c>
       <c r="B11" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16381" s="31" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="L12" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="C11" s="26" t="s">
-        <v>123</v>
+    </row>
+    <row r="13" spans="1:16381" s="27" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="29" t="s">
+        <v>99</v>
       </c>
-      <c r="D11" s="27" t="s">
-        <v>128</v>
+      <c r="B13" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="L13" s="26" t="s">
+        <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:16384" s="32" customFormat="1" ht="45" customHeight="1" thickBot="1">
-      <c r="A12" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="D12" s="32" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16384" s="27" customFormat="1" ht="75" customHeight="1" thickBot="1">
-      <c r="A13" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16384" s="25" customFormat="1"/>
-    <row r="15" spans="1:16384" s="25" customFormat="1" ht="15" thickBot="1">
+    <row r="14" spans="1:16381" s="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:16381" s="25" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
@@ -18537,28 +18504,25 @@
       <c r="XEY15"/>
       <c r="XEZ15"/>
       <c r="XFA15"/>
-      <c r="XFB15"/>
-      <c r="XFC15"/>
-      <c r="XFD15"/>
     </row>
-    <row r="16" spans="1:16384" ht="15" thickBot="1">
+    <row r="16" spans="1:16381" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15" thickBot="1">
+    <row r="19" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -18567,7 +18531,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>